<commit_message>
Added more features in ETL. Added more parameters for Hyperparam search
</commit_message>
<xml_diff>
--- a/datasets/interim/query_generator.xlsx
+++ b/datasets/interim/query_generator.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uribe/Documents/Code/University/2do_Cuatri/DM_EyF/DMEyF-2023-Ultima-Kaggle/datasets/interim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC84F58-AA4A-AC4F-B063-3BE23A8E03EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0041F186-1F7A-EC44-A408-912BA70B99A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36000" yWindow="-1240" windowWidth="51200" windowHeight="21100" xr2:uid="{B3A4B4EE-7E24-E74A-9ED8-7D85267AC8B6}"/>
+    <workbookView xWindow="61600" yWindow="-1240" windowWidth="25600" windowHeight="21100" xr2:uid="{B3A4B4EE-7E24-E74A-9ED8-7D85267AC8B6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="LAGS_DELTA_LAGS" sheetId="1" r:id="rId1"/>
+    <sheet name="MEDIA_MOVIL" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="154">
   <si>
     <t>active_quarter</t>
   </si>
@@ -854,8 +855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10D9082C-AFFA-A94A-88D4-CE7E9F295F15}">
   <dimension ref="A1:J153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
-      <selection activeCell="B160" sqref="B160"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7119,4 +7120,3228 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F91BE958-2715-A242-8587-47435FAF6544}">
+  <dimension ref="A1:E153"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="188.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B1" s="1">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="str">
+        <f>_xlfn.CONCAT($A2,"_avg_",B$1)</f>
+        <v>active_quarter_avg_3</v>
+      </c>
+      <c r="C2" t="str">
+        <f t="shared" ref="C2:C17" si="0">_xlfn.CONCAT($A2,"_avg_",C$1)</f>
+        <v>active_quarter_avg_6</v>
+      </c>
+      <c r="D2" t="str">
+        <f>",AVG(" &amp;$A2 &amp;", " &amp;B$1 &amp;") OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN " &amp;B$1 &amp; " PRECEDING AND CURRENT ROW) AS " &amp;B2</f>
+        <v>,AVG(active_quarter, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS active_quarter_avg_3</v>
+      </c>
+      <c r="E2" t="str">
+        <f>",AVG(" &amp;$A2 &amp;", " &amp;C$1 &amp;") OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN " &amp;C$1 &amp; " PRECEDING AND CURRENT ROW) AS " &amp;C2</f>
+        <v>,AVG(active_quarter, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS active_quarter_avg_6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:C34" si="1">_xlfn.CONCAT($A3,"_avg_",B$1)</f>
+        <v>catm_trx_avg_3</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" si="0"/>
+        <v>catm_trx_avg_6</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:E66" si="2">",AVG(" &amp;$A3 &amp;", " &amp;B$1 &amp;") OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN " &amp;B$1 &amp; " PRECEDING AND CURRENT ROW) AS " &amp;B3</f>
+        <v>,AVG(catm_trx, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS catm_trx_avg_3</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(catm_trx, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS catm_trx_avg_6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="1"/>
+        <v>catm_trx_other_avg_3</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>catm_trx_other_avg_6</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(catm_trx_other, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS catm_trx_other_avg_3</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(catm_trx_other, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS catm_trx_other_avg_6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="1"/>
+        <v>ccaja_ahorro_avg_3</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>ccaja_ahorro_avg_6</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ccaja_ahorro, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS ccaja_ahorro_avg_3</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ccaja_ahorro, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS ccaja_ahorro_avg_6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="1"/>
+        <v>ccaja_seguridad_avg_3</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>ccaja_seguridad_avg_6</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ccaja_seguridad, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS ccaja_seguridad_avg_3</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ccaja_seguridad, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS ccaja_seguridad_avg_6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="1"/>
+        <v>ccajas_consultas_avg_3</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>ccajas_consultas_avg_6</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ccajas_consultas, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS ccajas_consultas_avg_3</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ccajas_consultas, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS ccajas_consultas_avg_6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="1"/>
+        <v>ccajas_depositos_avg_3</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>ccajas_depositos_avg_6</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ccajas_depositos, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS ccajas_depositos_avg_3</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ccajas_depositos, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS ccajas_depositos_avg_6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="1"/>
+        <v>ccajas_extracciones_avg_3</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>ccajas_extracciones_avg_6</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ccajas_extracciones, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS ccajas_extracciones_avg_3</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ccajas_extracciones, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS ccajas_extracciones_avg_6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="1"/>
+        <v>ccajas_otras_avg_3</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>ccajas_otras_avg_6</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ccajas_otras, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS ccajas_otras_avg_3</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ccajas_otras, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS ccajas_otras_avg_6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="1"/>
+        <v>ccajas_transacciones_avg_3</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>ccajas_transacciones_avg_6</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ccajas_transacciones, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS ccajas_transacciones_avg_3</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ccajas_transacciones, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS ccajas_transacciones_avg_6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="1"/>
+        <v>ccajeros_propios_descuentos_avg_3</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>ccajeros_propios_descuentos_avg_6</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ccajeros_propios_descuentos, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS ccajeros_propios_descuentos_avg_3</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ccajeros_propios_descuentos, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS ccajeros_propios_descuentos_avg_6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="1"/>
+        <v>ccallcenter_transacciones_avg_3</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>ccallcenter_transacciones_avg_6</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ccallcenter_transacciones, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS ccallcenter_transacciones_avg_3</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ccallcenter_transacciones, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS ccallcenter_transacciones_avg_6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="1"/>
+        <v>ccheques_depositados_avg_3</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>ccheques_depositados_avg_6</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ccheques_depositados, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS ccheques_depositados_avg_3</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ccheques_depositados, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS ccheques_depositados_avg_6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="1"/>
+        <v>ccheques_depositados_rechazados_avg_3</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>ccheques_depositados_rechazados_avg_6</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ccheques_depositados_rechazados, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS ccheques_depositados_rechazados_avg_3</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ccheques_depositados_rechazados, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS ccheques_depositados_rechazados_avg_6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="1"/>
+        <v>ccheques_emitidos_avg_3</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>ccheques_emitidos_avg_6</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ccheques_emitidos, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS ccheques_emitidos_avg_3</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ccheques_emitidos, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS ccheques_emitidos_avg_6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="1"/>
+        <v>ccheques_emitidos_rechazados_avg_3</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>ccheques_emitidos_rechazados_avg_6</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ccheques_emitidos_rechazados, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS ccheques_emitidos_rechazados_avg_3</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ccheques_emitidos_rechazados, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS ccheques_emitidos_rechazados_avg_6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="1"/>
+        <v>ccomisiones_mantenimiento_avg_3</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="1"/>
+        <v>ccomisiones_mantenimiento_avg_6</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ccomisiones_mantenimiento, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS ccomisiones_mantenimiento_avg_3</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ccomisiones_mantenimiento, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS ccomisiones_mantenimiento_avg_6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="1"/>
+        <v>ccomisiones_otras_avg_3</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="1"/>
+        <v>ccomisiones_otras_avg_6</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ccomisiones_otras, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS ccomisiones_otras_avg_3</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ccomisiones_otras, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS ccomisiones_otras_avg_6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="1"/>
+        <v>ccuenta_corriente_avg_3</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="1"/>
+        <v>ccuenta_corriente_avg_6</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ccuenta_corriente, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS ccuenta_corriente_avg_3</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ccuenta_corriente, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS ccuenta_corriente_avg_6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="1"/>
+        <v>ccuenta_debitos_automaticos_avg_3</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="1"/>
+        <v>ccuenta_debitos_automaticos_avg_6</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ccuenta_debitos_automaticos, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS ccuenta_debitos_automaticos_avg_3</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ccuenta_debitos_automaticos, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS ccuenta_debitos_automaticos_avg_6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" si="1"/>
+        <v>cdescubierto_preacordado_avg_3</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="1"/>
+        <v>cdescubierto_preacordado_avg_6</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cdescubierto_preacordado, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS cdescubierto_preacordado_avg_3</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cdescubierto_preacordado, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS cdescubierto_preacordado_avg_6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" si="1"/>
+        <v>cextraccion_autoservicio_avg_3</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="1"/>
+        <v>cextraccion_autoservicio_avg_6</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cextraccion_autoservicio, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS cextraccion_autoservicio_avg_3</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cextraccion_autoservicio, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS cextraccion_autoservicio_avg_6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" si="1"/>
+        <v>cforex_avg_3</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="1"/>
+        <v>cforex_avg_6</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cforex, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS cforex_avg_3</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cforex, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS cforex_avg_6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="1"/>
+        <v>cforex_buy_avg_3</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="1"/>
+        <v>cforex_buy_avg_6</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cforex_buy, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS cforex_buy_avg_3</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cforex_buy, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS cforex_buy_avg_6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" t="str">
+        <f t="shared" si="1"/>
+        <v>cforex_sell_avg_3</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="1"/>
+        <v>cforex_sell_avg_6</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cforex_sell, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS cforex_sell_avg_3</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cforex_sell, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS cforex_sell_avg_6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>95</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" si="1"/>
+        <v>chomebanking_transacciones_avg_3</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="1"/>
+        <v>chomebanking_transacciones_avg_6</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(chomebanking_transacciones, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS chomebanking_transacciones_avg_3</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(chomebanking_transacciones, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS chomebanking_transacciones_avg_6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" si="1"/>
+        <v>cinversion1_avg_3</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="1"/>
+        <v>cinversion1_avg_6</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cinversion1, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS cinversion1_avg_3</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cinversion1, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS cinversion1_avg_6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" t="str">
+        <f t="shared" si="1"/>
+        <v>cinversion2_avg_3</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="1"/>
+        <v>cinversion2_avg_6</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cinversion2, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS cinversion2_avg_3</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cinversion2, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS cinversion2_avg_6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" t="str">
+        <f t="shared" si="1"/>
+        <v>cliente_antiguedad_avg_3</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="1"/>
+        <v>cliente_antiguedad_avg_6</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cliente_antiguedad, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS cliente_antiguedad_avg_3</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cliente_antiguedad, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS cliente_antiguedad_avg_6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" t="str">
+        <f t="shared" si="1"/>
+        <v>cliente_edad_avg_3</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="1"/>
+        <v>cliente_edad_avg_6</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cliente_edad, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS cliente_edad_avg_3</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cliente_edad, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS cliente_edad_avg_6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" t="str">
+        <f t="shared" si="1"/>
+        <v>cliente_vip_avg_3</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="1"/>
+        <v>cliente_vip_avg_6</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cliente_vip, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS cliente_vip_avg_3</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cliente_vip, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS cliente_vip_avg_6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>107</v>
+      </c>
+      <c r="B33" t="str">
+        <f t="shared" si="1"/>
+        <v>cmobile_app_trx_avg_3</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="1"/>
+        <v>cmobile_app_trx_avg_6</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cmobile_app_trx, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS cmobile_app_trx_avg_3</v>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cmobile_app_trx, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS cmobile_app_trx_avg_6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" t="str">
+        <f t="shared" si="1"/>
+        <v>cpagodeservicios_avg_3</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="1"/>
+        <v>cpagodeservicios_avg_6</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cpagodeservicios, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS cpagodeservicios_avg_3</v>
+      </c>
+      <c r="E34" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cpagodeservicios, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS cpagodeservicios_avg_6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" t="str">
+        <f t="shared" ref="B35:C66" si="3">_xlfn.CONCAT($A35,"_avg_",B$1)</f>
+        <v>cpagomiscuentas_avg_3</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="3"/>
+        <v>cpagomiscuentas_avg_6</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cpagomiscuentas, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS cpagomiscuentas_avg_3</v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cpagomiscuentas, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS cpagomiscuentas_avg_6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" t="str">
+        <f t="shared" si="3"/>
+        <v>cpayroll2_trx_avg_3</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="3"/>
+        <v>cpayroll2_trx_avg_6</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cpayroll2_trx, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS cpayroll2_trx_avg_3</v>
+      </c>
+      <c r="E36" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cpayroll2_trx, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS cpayroll2_trx_avg_6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" t="str">
+        <f t="shared" si="3"/>
+        <v>cpayroll_trx_avg_3</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="3"/>
+        <v>cpayroll_trx_avg_6</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cpayroll_trx, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS cpayroll_trx_avg_3</v>
+      </c>
+      <c r="E37" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cpayroll_trx, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS cpayroll_trx_avg_6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" t="str">
+        <f t="shared" si="3"/>
+        <v>cplazo_fijo_avg_3</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="3"/>
+        <v>cplazo_fijo_avg_6</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cplazo_fijo, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS cplazo_fijo_avg_3</v>
+      </c>
+      <c r="E38" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cplazo_fijo, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS cplazo_fijo_avg_6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" t="str">
+        <f t="shared" si="3"/>
+        <v>cprestamos_hipotecarios_avg_3</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="3"/>
+        <v>cprestamos_hipotecarios_avg_6</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cprestamos_hipotecarios, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS cprestamos_hipotecarios_avg_3</v>
+      </c>
+      <c r="E39" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cprestamos_hipotecarios, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS cprestamos_hipotecarios_avg_6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>30</v>
+      </c>
+      <c r="B40" t="str">
+        <f t="shared" si="3"/>
+        <v>cprestamos_personales_avg_3</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="3"/>
+        <v>cprestamos_personales_avg_6</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cprestamos_personales, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS cprestamos_personales_avg_3</v>
+      </c>
+      <c r="E40" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cprestamos_personales, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS cprestamos_personales_avg_6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>32</v>
+      </c>
+      <c r="B41" t="str">
+        <f t="shared" si="3"/>
+        <v>cprestamos_prendarios_avg_3</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" si="3"/>
+        <v>cprestamos_prendarios_avg_6</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cprestamos_prendarios, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS cprestamos_prendarios_avg_3</v>
+      </c>
+      <c r="E41" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cprestamos_prendarios, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS cprestamos_prendarios_avg_6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42" t="str">
+        <f t="shared" si="3"/>
+        <v>cproductos_avg_3</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" si="3"/>
+        <v>cproductos_avg_6</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cproductos, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS cproductos_avg_3</v>
+      </c>
+      <c r="E42" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cproductos, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS cproductos_avg_6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>47</v>
+      </c>
+      <c r="B43" t="str">
+        <f t="shared" si="3"/>
+        <v>cseguro_accidentes_personales_avg_3</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" si="3"/>
+        <v>cseguro_accidentes_personales_avg_6</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cseguro_accidentes_personales, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS cseguro_accidentes_personales_avg_3</v>
+      </c>
+      <c r="E43" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cseguro_accidentes_personales, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS cseguro_accidentes_personales_avg_6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44" t="str">
+        <f t="shared" si="3"/>
+        <v>cseguro_auto_avg_3</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" si="3"/>
+        <v>cseguro_auto_avg_6</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cseguro_auto, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS cseguro_auto_avg_3</v>
+      </c>
+      <c r="E44" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cseguro_auto, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS cseguro_auto_avg_6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" t="str">
+        <f t="shared" si="3"/>
+        <v>cseguro_vida_avg_3</v>
+      </c>
+      <c r="C45" t="str">
+        <f t="shared" si="3"/>
+        <v>cseguro_vida_avg_6</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cseguro_vida, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS cseguro_vida_avg_3</v>
+      </c>
+      <c r="E45" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cseguro_vida, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS cseguro_vida_avg_6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46" t="str">
+        <f t="shared" si="3"/>
+        <v>cseguro_vivienda_avg_3</v>
+      </c>
+      <c r="C46" t="str">
+        <f t="shared" si="3"/>
+        <v>cseguro_vivienda_avg_6</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cseguro_vivienda, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS cseguro_vivienda_avg_3</v>
+      </c>
+      <c r="E46" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(cseguro_vivienda, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS cseguro_vivienda_avg_6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>21</v>
+      </c>
+      <c r="B47" t="str">
+        <f t="shared" si="3"/>
+        <v>ctarjeta_debito_avg_3</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" si="3"/>
+        <v>ctarjeta_debito_avg_6</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ctarjeta_debito, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS ctarjeta_debito_avg_3</v>
+      </c>
+      <c r="E47" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ctarjeta_debito, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS ctarjeta_debito_avg_6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>22</v>
+      </c>
+      <c r="B48" t="str">
+        <f t="shared" si="3"/>
+        <v>ctarjeta_debito_transacciones_avg_3</v>
+      </c>
+      <c r="C48" t="str">
+        <f t="shared" si="3"/>
+        <v>ctarjeta_debito_transacciones_avg_6</v>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ctarjeta_debito_transacciones, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS ctarjeta_debito_transacciones_avg_3</v>
+      </c>
+      <c r="E48" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ctarjeta_debito_transacciones, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS ctarjeta_debito_transacciones_avg_6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>27</v>
+      </c>
+      <c r="B49" t="str">
+        <f t="shared" si="3"/>
+        <v>ctarjeta_master_avg_3</v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" si="3"/>
+        <v>ctarjeta_master_avg_6</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ctarjeta_master, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS ctarjeta_master_avg_3</v>
+      </c>
+      <c r="E49" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ctarjeta_master, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS ctarjeta_master_avg_6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>57</v>
+      </c>
+      <c r="B50" t="str">
+        <f t="shared" si="3"/>
+        <v>ctarjeta_master_debitos_automaticos_avg_3</v>
+      </c>
+      <c r="C50" t="str">
+        <f t="shared" si="3"/>
+        <v>ctarjeta_master_debitos_automaticos_avg_6</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ctarjeta_master_debitos_automaticos, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS ctarjeta_master_debitos_automaticos_avg_3</v>
+      </c>
+      <c r="E50" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ctarjeta_master_debitos_automaticos, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS ctarjeta_master_debitos_automaticos_avg_6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>67</v>
+      </c>
+      <c r="B51" t="str">
+        <f t="shared" si="3"/>
+        <v>ctarjeta_master_descuentos_avg_3</v>
+      </c>
+      <c r="C51" t="str">
+        <f t="shared" si="3"/>
+        <v>ctarjeta_master_descuentos_avg_6</v>
+      </c>
+      <c r="D51" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ctarjeta_master_descuentos, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS ctarjeta_master_descuentos_avg_3</v>
+      </c>
+      <c r="E51" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ctarjeta_master_descuentos, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS ctarjeta_master_descuentos_avg_6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>28</v>
+      </c>
+      <c r="B52" t="str">
+        <f t="shared" si="3"/>
+        <v>ctarjeta_master_transacciones_avg_3</v>
+      </c>
+      <c r="C52" t="str">
+        <f t="shared" si="3"/>
+        <v>ctarjeta_master_transacciones_avg_6</v>
+      </c>
+      <c r="D52" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ctarjeta_master_transacciones, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS ctarjeta_master_transacciones_avg_3</v>
+      </c>
+      <c r="E52" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ctarjeta_master_transacciones, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS ctarjeta_master_transacciones_avg_6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>24</v>
+      </c>
+      <c r="B53" t="str">
+        <f t="shared" si="3"/>
+        <v>ctarjeta_visa_avg_3</v>
+      </c>
+      <c r="C53" t="str">
+        <f t="shared" si="3"/>
+        <v>ctarjeta_visa_avg_6</v>
+      </c>
+      <c r="D53" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ctarjeta_visa, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS ctarjeta_visa_avg_3</v>
+      </c>
+      <c r="E53" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ctarjeta_visa, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS ctarjeta_visa_avg_6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>55</v>
+      </c>
+      <c r="B54" t="str">
+        <f t="shared" si="3"/>
+        <v>ctarjeta_visa_debitos_automaticos_avg_3</v>
+      </c>
+      <c r="C54" t="str">
+        <f t="shared" si="3"/>
+        <v>ctarjeta_visa_debitos_automaticos_avg_6</v>
+      </c>
+      <c r="D54" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ctarjeta_visa_debitos_automaticos, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS ctarjeta_visa_debitos_automaticos_avg_3</v>
+      </c>
+      <c r="E54" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ctarjeta_visa_debitos_automaticos, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS ctarjeta_visa_debitos_automaticos_avg_6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>65</v>
+      </c>
+      <c r="B55" t="str">
+        <f t="shared" si="3"/>
+        <v>ctarjeta_visa_descuentos_avg_3</v>
+      </c>
+      <c r="C55" t="str">
+        <f t="shared" si="3"/>
+        <v>ctarjeta_visa_descuentos_avg_6</v>
+      </c>
+      <c r="D55" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ctarjeta_visa_descuentos, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS ctarjeta_visa_descuentos_avg_3</v>
+      </c>
+      <c r="E55" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ctarjeta_visa_descuentos, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS ctarjeta_visa_descuentos_avg_6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>25</v>
+      </c>
+      <c r="B56" t="str">
+        <f t="shared" si="3"/>
+        <v>ctarjeta_visa_transacciones_avg_3</v>
+      </c>
+      <c r="C56" t="str">
+        <f t="shared" si="3"/>
+        <v>ctarjeta_visa_transacciones_avg_6</v>
+      </c>
+      <c r="D56" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ctarjeta_visa_transacciones, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS ctarjeta_visa_transacciones_avg_3</v>
+      </c>
+      <c r="E56" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ctarjeta_visa_transacciones, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS ctarjeta_visa_transacciones_avg_6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>80</v>
+      </c>
+      <c r="B57" t="str">
+        <f t="shared" si="3"/>
+        <v>ctransferencias_emitidas_avg_3</v>
+      </c>
+      <c r="C57" t="str">
+        <f t="shared" si="3"/>
+        <v>ctransferencias_emitidas_avg_6</v>
+      </c>
+      <c r="D57" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ctransferencias_emitidas, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS ctransferencias_emitidas_avg_3</v>
+      </c>
+      <c r="E57" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ctransferencias_emitidas, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS ctransferencias_emitidas_avg_6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>78</v>
+      </c>
+      <c r="B58" t="str">
+        <f t="shared" si="3"/>
+        <v>ctransferencias_recibidas_avg_3</v>
+      </c>
+      <c r="C58" t="str">
+        <f t="shared" si="3"/>
+        <v>ctransferencias_recibidas_avg_6</v>
+      </c>
+      <c r="D58" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ctransferencias_recibidas, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS ctransferencias_recibidas_avg_3</v>
+      </c>
+      <c r="E58" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ctransferencias_recibidas, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS ctransferencias_recibidas_avg_6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>105</v>
+      </c>
+      <c r="B59" t="str">
+        <f t="shared" si="3"/>
+        <v>ctrx_quarter_avg_3</v>
+      </c>
+      <c r="C59" t="str">
+        <f t="shared" si="3"/>
+        <v>ctrx_quarter_avg_6</v>
+      </c>
+      <c r="D59" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ctrx_quarter, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS ctrx_quarter_avg_3</v>
+      </c>
+      <c r="E59" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(ctrx_quarter, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS ctrx_quarter_avg_6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>2</v>
+      </c>
+      <c r="B60" t="str">
+        <f t="shared" si="3"/>
+        <v>internet_avg_3</v>
+      </c>
+      <c r="C60" t="str">
+        <f t="shared" si="3"/>
+        <v>internet_avg_6</v>
+      </c>
+      <c r="D60" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(internet, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS internet_avg_3</v>
+      </c>
+      <c r="E60" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(internet, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS internet_avg_6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>8</v>
+      </c>
+      <c r="B61" t="str">
+        <f t="shared" si="3"/>
+        <v>mactivos_margen_avg_3</v>
+      </c>
+      <c r="C61" t="str">
+        <f t="shared" si="3"/>
+        <v>mactivos_margen_avg_6</v>
+      </c>
+      <c r="D61" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(mactivos_margen, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS mactivos_margen_avg_3</v>
+      </c>
+      <c r="E61" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(mactivos_margen, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS mactivos_margen_avg_6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>128</v>
+      </c>
+      <c r="B62" t="str">
+        <f t="shared" si="3"/>
+        <v>Master_cadelantosefectivo_avg_3</v>
+      </c>
+      <c r="C62" t="str">
+        <f t="shared" si="3"/>
+        <v>Master_cadelantosefectivo_avg_6</v>
+      </c>
+      <c r="D62" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(Master_cadelantosefectivo, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Master_cadelantosefectivo_avg_3</v>
+      </c>
+      <c r="E62" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(Master_cadelantosefectivo, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Master_cadelantosefectivo_avg_6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>127</v>
+      </c>
+      <c r="B63" t="str">
+        <f t="shared" si="3"/>
+        <v>Master_cconsumos_avg_3</v>
+      </c>
+      <c r="C63" t="str">
+        <f t="shared" si="3"/>
+        <v>Master_cconsumos_avg_6</v>
+      </c>
+      <c r="D63" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(Master_cconsumos, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Master_cconsumos_avg_3</v>
+      </c>
+      <c r="E63" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(Master_cconsumos, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Master_cconsumos_avg_6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>108</v>
+      </c>
+      <c r="B64" t="str">
+        <f t="shared" si="3"/>
+        <v>Master_delinquency_avg_3</v>
+      </c>
+      <c r="C64" t="str">
+        <f t="shared" si="3"/>
+        <v>Master_delinquency_avg_6</v>
+      </c>
+      <c r="D64" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(Master_delinquency, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Master_delinquency_avg_3</v>
+      </c>
+      <c r="E64" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(Master_delinquency, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Master_delinquency_avg_6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>125</v>
+      </c>
+      <c r="B65" t="str">
+        <f t="shared" si="3"/>
+        <v>Master_fechaalta_avg_3</v>
+      </c>
+      <c r="C65" t="str">
+        <f t="shared" si="3"/>
+        <v>Master_fechaalta_avg_6</v>
+      </c>
+      <c r="D65" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(Master_fechaalta, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Master_fechaalta_avg_3</v>
+      </c>
+      <c r="E65" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(Master_fechaalta, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Master_fechaalta_avg_6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>112</v>
+      </c>
+      <c r="B66" t="str">
+        <f t="shared" si="3"/>
+        <v>Master_Finiciomora_avg_3</v>
+      </c>
+      <c r="C66" t="str">
+        <f t="shared" si="3"/>
+        <v>Master_Finiciomora_avg_6</v>
+      </c>
+      <c r="D66" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(Master_Finiciomora, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Master_Finiciomora_avg_3</v>
+      </c>
+      <c r="E66" t="str">
+        <f t="shared" si="2"/>
+        <v>,AVG(Master_Finiciomora, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Master_Finiciomora_avg_6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>121</v>
+      </c>
+      <c r="B67" t="str">
+        <f t="shared" ref="B67:C98" si="4">_xlfn.CONCAT($A67,"_avg_",B$1)</f>
+        <v>Master_fultimo_cierre_avg_3</v>
+      </c>
+      <c r="C67" t="str">
+        <f t="shared" si="4"/>
+        <v>Master_fultimo_cierre_avg_6</v>
+      </c>
+      <c r="D67" t="str">
+        <f t="shared" ref="D67:E130" si="5">",AVG(" &amp;$A67 &amp;", " &amp;B$1 &amp;") OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN " &amp;B$1 &amp; " PRECEDING AND CURRENT ROW) AS " &amp;B67</f>
+        <v>,AVG(Master_fultimo_cierre, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Master_fultimo_cierre_avg_3</v>
+      </c>
+      <c r="E67" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(Master_fultimo_cierre, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Master_fultimo_cierre_avg_6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>111</v>
+      </c>
+      <c r="B68" t="str">
+        <f t="shared" si="4"/>
+        <v>Master_Fvencimiento_avg_3</v>
+      </c>
+      <c r="C68" t="str">
+        <f t="shared" si="4"/>
+        <v>Master_Fvencimiento_avg_6</v>
+      </c>
+      <c r="D68" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(Master_Fvencimiento, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Master_Fvencimiento_avg_3</v>
+      </c>
+      <c r="E68" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(Master_Fvencimiento, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Master_Fvencimiento_avg_6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>120</v>
+      </c>
+      <c r="B69" t="str">
+        <f t="shared" si="4"/>
+        <v>Master_madelantodolares_avg_3</v>
+      </c>
+      <c r="C69" t="str">
+        <f t="shared" si="4"/>
+        <v>Master_madelantodolares_avg_6</v>
+      </c>
+      <c r="D69" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(Master_madelantodolares, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Master_madelantodolares_avg_3</v>
+      </c>
+      <c r="E69" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(Master_madelantodolares, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Master_madelantodolares_avg_6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>119</v>
+      </c>
+      <c r="B70" t="str">
+        <f t="shared" si="4"/>
+        <v>Master_madelantopesos_avg_3</v>
+      </c>
+      <c r="C70" t="str">
+        <f t="shared" si="4"/>
+        <v>Master_madelantopesos_avg_6</v>
+      </c>
+      <c r="D70" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(Master_madelantopesos, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Master_madelantopesos_avg_3</v>
+      </c>
+      <c r="E70" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(Master_madelantopesos, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Master_madelantopesos_avg_6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>117</v>
+      </c>
+      <c r="B71" t="str">
+        <f t="shared" si="4"/>
+        <v>Master_mconsumosdolares_avg_3</v>
+      </c>
+      <c r="C71" t="str">
+        <f t="shared" si="4"/>
+        <v>Master_mconsumosdolares_avg_6</v>
+      </c>
+      <c r="D71" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(Master_mconsumosdolares, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Master_mconsumosdolares_avg_3</v>
+      </c>
+      <c r="E71" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(Master_mconsumosdolares, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Master_mconsumosdolares_avg_6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>116</v>
+      </c>
+      <c r="B72" t="str">
+        <f t="shared" si="4"/>
+        <v>Master_mconsumospesos_avg_3</v>
+      </c>
+      <c r="C72" t="str">
+        <f t="shared" si="4"/>
+        <v>Master_mconsumospesos_avg_6</v>
+      </c>
+      <c r="D72" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(Master_mconsumospesos, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Master_mconsumospesos_avg_3</v>
+      </c>
+      <c r="E72" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(Master_mconsumospesos, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Master_mconsumospesos_avg_6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>126</v>
+      </c>
+      <c r="B73" t="str">
+        <f t="shared" si="4"/>
+        <v>Master_mconsumototal_avg_3</v>
+      </c>
+      <c r="C73" t="str">
+        <f t="shared" si="4"/>
+        <v>Master_mconsumototal_avg_6</v>
+      </c>
+      <c r="D73" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(Master_mconsumototal, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Master_mconsumototal_avg_3</v>
+      </c>
+      <c r="E73" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(Master_mconsumototal, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Master_mconsumototal_avg_6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>110</v>
+      </c>
+      <c r="B74" t="str">
+        <f t="shared" si="4"/>
+        <v>Master_mfinanciacion_limite_avg_3</v>
+      </c>
+      <c r="C74" t="str">
+        <f t="shared" si="4"/>
+        <v>Master_mfinanciacion_limite_avg_6</v>
+      </c>
+      <c r="D74" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(Master_mfinanciacion_limite, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Master_mfinanciacion_limite_avg_3</v>
+      </c>
+      <c r="E74" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(Master_mfinanciacion_limite, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Master_mfinanciacion_limite_avg_6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>118</v>
+      </c>
+      <c r="B75" t="str">
+        <f t="shared" si="4"/>
+        <v>Master_mlimitecompra_avg_3</v>
+      </c>
+      <c r="C75" t="str">
+        <f t="shared" si="4"/>
+        <v>Master_mlimitecompra_avg_6</v>
+      </c>
+      <c r="D75" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(Master_mlimitecompra, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Master_mlimitecompra_avg_3</v>
+      </c>
+      <c r="E75" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(Master_mlimitecompra, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Master_mlimitecompra_avg_6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>122</v>
+      </c>
+      <c r="B76" t="str">
+        <f t="shared" si="4"/>
+        <v>Master_mpagado_avg_3</v>
+      </c>
+      <c r="C76" t="str">
+        <f t="shared" si="4"/>
+        <v>Master_mpagado_avg_6</v>
+      </c>
+      <c r="D76" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(Master_mpagado, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Master_mpagado_avg_3</v>
+      </c>
+      <c r="E76" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(Master_mpagado, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Master_mpagado_avg_6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>129</v>
+      </c>
+      <c r="B77" t="str">
+        <f t="shared" si="4"/>
+        <v>Master_mpagominimo_avg_3</v>
+      </c>
+      <c r="C77" t="str">
+        <f t="shared" si="4"/>
+        <v>Master_mpagominimo_avg_6</v>
+      </c>
+      <c r="D77" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(Master_mpagominimo, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Master_mpagominimo_avg_3</v>
+      </c>
+      <c r="E77" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(Master_mpagominimo, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Master_mpagominimo_avg_6</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>124</v>
+      </c>
+      <c r="B78" t="str">
+        <f t="shared" si="4"/>
+        <v>Master_mpagosdolares_avg_3</v>
+      </c>
+      <c r="C78" t="str">
+        <f t="shared" si="4"/>
+        <v>Master_mpagosdolares_avg_6</v>
+      </c>
+      <c r="D78" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(Master_mpagosdolares, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Master_mpagosdolares_avg_3</v>
+      </c>
+      <c r="E78" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(Master_mpagosdolares, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Master_mpagosdolares_avg_6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>123</v>
+      </c>
+      <c r="B79" t="str">
+        <f t="shared" si="4"/>
+        <v>Master_mpagospesos_avg_3</v>
+      </c>
+      <c r="C79" t="str">
+        <f t="shared" si="4"/>
+        <v>Master_mpagospesos_avg_6</v>
+      </c>
+      <c r="D79" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(Master_mpagospesos, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Master_mpagospesos_avg_3</v>
+      </c>
+      <c r="E79" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(Master_mpagospesos, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Master_mpagospesos_avg_6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>115</v>
+      </c>
+      <c r="B80" t="str">
+        <f t="shared" si="4"/>
+        <v>Master_msaldodolares_avg_3</v>
+      </c>
+      <c r="C80" t="str">
+        <f t="shared" si="4"/>
+        <v>Master_msaldodolares_avg_6</v>
+      </c>
+      <c r="D80" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(Master_msaldodolares, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Master_msaldodolares_avg_3</v>
+      </c>
+      <c r="E80" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(Master_msaldodolares, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Master_msaldodolares_avg_6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>114</v>
+      </c>
+      <c r="B81" t="str">
+        <f t="shared" si="4"/>
+        <v>Master_msaldopesos_avg_3</v>
+      </c>
+      <c r="C81" t="str">
+        <f t="shared" si="4"/>
+        <v>Master_msaldopesos_avg_6</v>
+      </c>
+      <c r="D81" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(Master_msaldopesos, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Master_msaldopesos_avg_3</v>
+      </c>
+      <c r="E81" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(Master_msaldopesos, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Master_msaldopesos_avg_6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>113</v>
+      </c>
+      <c r="B82" t="str">
+        <f t="shared" si="4"/>
+        <v>Master_msaldototal_avg_3</v>
+      </c>
+      <c r="C82" t="str">
+        <f t="shared" si="4"/>
+        <v>Master_msaldototal_avg_6</v>
+      </c>
+      <c r="D82" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(Master_msaldototal, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Master_msaldototal_avg_3</v>
+      </c>
+      <c r="E82" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(Master_msaldototal, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Master_msaldototal_avg_6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>109</v>
+      </c>
+      <c r="B83" t="str">
+        <f t="shared" si="4"/>
+        <v>Master_status_avg_3</v>
+      </c>
+      <c r="C83" t="str">
+        <f t="shared" si="4"/>
+        <v>Master_status_avg_6</v>
+      </c>
+      <c r="D83" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(Master_status, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Master_status_avg_3</v>
+      </c>
+      <c r="E83" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(Master_status, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Master_status_avg_6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>102</v>
+      </c>
+      <c r="B84" t="str">
+        <f t="shared" si="4"/>
+        <v>matm_avg_3</v>
+      </c>
+      <c r="C84" t="str">
+        <f t="shared" si="4"/>
+        <v>matm_avg_6</v>
+      </c>
+      <c r="D84" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(matm, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS matm_avg_3</v>
+      </c>
+      <c r="E84" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(matm, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS matm_avg_6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>104</v>
+      </c>
+      <c r="B85" t="str">
+        <f t="shared" si="4"/>
+        <v>matm_other_avg_3</v>
+      </c>
+      <c r="C85" t="str">
+        <f t="shared" si="4"/>
+        <v>matm_other_avg_6</v>
+      </c>
+      <c r="D85" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(matm_other, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS matm_other_avg_3</v>
+      </c>
+      <c r="E85" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(matm_other, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS matm_other_avg_6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>23</v>
+      </c>
+      <c r="B86" t="str">
+        <f t="shared" si="4"/>
+        <v>mautoservicio_avg_3</v>
+      </c>
+      <c r="C86" t="str">
+        <f t="shared" si="4"/>
+        <v>mautoservicio_avg_6</v>
+      </c>
+      <c r="D86" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mautoservicio, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS mautoservicio_avg_3</v>
+      </c>
+      <c r="E86" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mautoservicio, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS mautoservicio_avg_6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>16</v>
+      </c>
+      <c r="B87" t="str">
+        <f t="shared" si="4"/>
+        <v>mcaja_ahorro_avg_3</v>
+      </c>
+      <c r="C87" t="str">
+        <f t="shared" si="4"/>
+        <v>mcaja_ahorro_avg_6</v>
+      </c>
+      <c r="D87" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mcaja_ahorro, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS mcaja_ahorro_avg_3</v>
+      </c>
+      <c r="E87" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mcaja_ahorro, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS mcaja_ahorro_avg_6</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>17</v>
+      </c>
+      <c r="B88" t="str">
+        <f t="shared" si="4"/>
+        <v>mcaja_ahorro_adicional_avg_3</v>
+      </c>
+      <c r="C88" t="str">
+        <f t="shared" si="4"/>
+        <v>mcaja_ahorro_adicional_avg_6</v>
+      </c>
+      <c r="D88" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mcaja_ahorro_adicional, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS mcaja_ahorro_adicional_avg_3</v>
+      </c>
+      <c r="E88" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mcaja_ahorro_adicional, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS mcaja_ahorro_adicional_avg_6</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>18</v>
+      </c>
+      <c r="B89" t="str">
+        <f t="shared" si="4"/>
+        <v>mcaja_ahorro_dolares_avg_3</v>
+      </c>
+      <c r="C89" t="str">
+        <f t="shared" si="4"/>
+        <v>mcaja_ahorro_dolares_avg_6</v>
+      </c>
+      <c r="D89" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mcaja_ahorro_dolares, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS mcaja_ahorro_dolares_avg_3</v>
+      </c>
+      <c r="E89" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mcaja_ahorro_dolares, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS mcaja_ahorro_dolares_avg_6</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>64</v>
+      </c>
+      <c r="B90" t="str">
+        <f t="shared" si="4"/>
+        <v>mcajeros_propios_descuentos_avg_3</v>
+      </c>
+      <c r="C90" t="str">
+        <f t="shared" si="4"/>
+        <v>mcajeros_propios_descuentos_avg_6</v>
+      </c>
+      <c r="D90" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mcajeros_propios_descuentos, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS mcajeros_propios_descuentos_avg_3</v>
+      </c>
+      <c r="E90" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mcajeros_propios_descuentos, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS mcajeros_propios_descuentos_avg_6</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>85</v>
+      </c>
+      <c r="B91" t="str">
+        <f t="shared" si="4"/>
+        <v>mcheques_depositados_avg_3</v>
+      </c>
+      <c r="C91" t="str">
+        <f t="shared" si="4"/>
+        <v>mcheques_depositados_avg_6</v>
+      </c>
+      <c r="D91" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mcheques_depositados, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS mcheques_depositados_avg_3</v>
+      </c>
+      <c r="E91" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mcheques_depositados, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS mcheques_depositados_avg_6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>89</v>
+      </c>
+      <c r="B92" t="str">
+        <f t="shared" si="4"/>
+        <v>mcheques_depositados_rechazados_avg_3</v>
+      </c>
+      <c r="C92" t="str">
+        <f t="shared" si="4"/>
+        <v>mcheques_depositados_rechazados_avg_6</v>
+      </c>
+      <c r="D92" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mcheques_depositados_rechazados, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS mcheques_depositados_rechazados_avg_3</v>
+      </c>
+      <c r="E92" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mcheques_depositados_rechazados, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS mcheques_depositados_rechazados_avg_6</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>87</v>
+      </c>
+      <c r="B93" t="str">
+        <f t="shared" si="4"/>
+        <v>mcheques_emitidos_avg_3</v>
+      </c>
+      <c r="C93" t="str">
+        <f t="shared" si="4"/>
+        <v>mcheques_emitidos_avg_6</v>
+      </c>
+      <c r="D93" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mcheques_emitidos, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS mcheques_emitidos_avg_3</v>
+      </c>
+      <c r="E93" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mcheques_emitidos, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS mcheques_emitidos_avg_6</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>91</v>
+      </c>
+      <c r="B94" t="str">
+        <f t="shared" si="4"/>
+        <v>mcheques_emitidos_rechazados_avg_3</v>
+      </c>
+      <c r="C94" t="str">
+        <f t="shared" si="4"/>
+        <v>mcheques_emitidos_rechazados_avg_6</v>
+      </c>
+      <c r="D94" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mcheques_emitidos_rechazados, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS mcheques_emitidos_rechazados_avg_3</v>
+      </c>
+      <c r="E94" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mcheques_emitidos_rechazados, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS mcheques_emitidos_rechazados_avg_6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>7</v>
+      </c>
+      <c r="B95" t="str">
+        <f t="shared" si="4"/>
+        <v>mcomisiones_avg_3</v>
+      </c>
+      <c r="C95" t="str">
+        <f t="shared" si="4"/>
+        <v>mcomisiones_avg_6</v>
+      </c>
+      <c r="D95" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mcomisiones, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS mcomisiones_avg_3</v>
+      </c>
+      <c r="E95" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mcomisiones, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS mcomisiones_avg_6</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>70</v>
+      </c>
+      <c r="B96" t="str">
+        <f t="shared" si="4"/>
+        <v>mcomisiones_mantenimiento_avg_3</v>
+      </c>
+      <c r="C96" t="str">
+        <f t="shared" si="4"/>
+        <v>mcomisiones_mantenimiento_avg_6</v>
+      </c>
+      <c r="D96" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mcomisiones_mantenimiento, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS mcomisiones_mantenimiento_avg_3</v>
+      </c>
+      <c r="E96" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mcomisiones_mantenimiento, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS mcomisiones_mantenimiento_avg_6</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>72</v>
+      </c>
+      <c r="B97" t="str">
+        <f t="shared" si="4"/>
+        <v>mcomisiones_otras_avg_3</v>
+      </c>
+      <c r="C97" t="str">
+        <f t="shared" si="4"/>
+        <v>mcomisiones_otras_avg_6</v>
+      </c>
+      <c r="D97" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mcomisiones_otras, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS mcomisiones_otras_avg_3</v>
+      </c>
+      <c r="E97" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mcomisiones_otras, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS mcomisiones_otras_avg_6</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>14</v>
+      </c>
+      <c r="B98" t="str">
+        <f t="shared" si="4"/>
+        <v>mcuenta_corriente_avg_3</v>
+      </c>
+      <c r="C98" t="str">
+        <f t="shared" si="4"/>
+        <v>mcuenta_corriente_avg_6</v>
+      </c>
+      <c r="D98" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mcuenta_corriente, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS mcuenta_corriente_avg_3</v>
+      </c>
+      <c r="E98" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mcuenta_corriente, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS mcuenta_corriente_avg_6</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>13</v>
+      </c>
+      <c r="B99" t="str">
+        <f t="shared" ref="B99:C130" si="6">_xlfn.CONCAT($A99,"_avg_",B$1)</f>
+        <v>mcuenta_corriente_adicional_avg_3</v>
+      </c>
+      <c r="C99" t="str">
+        <f t="shared" si="6"/>
+        <v>mcuenta_corriente_adicional_avg_6</v>
+      </c>
+      <c r="D99" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mcuenta_corriente_adicional, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS mcuenta_corriente_adicional_avg_3</v>
+      </c>
+      <c r="E99" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mcuenta_corriente_adicional, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS mcuenta_corriente_adicional_avg_6</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>54</v>
+      </c>
+      <c r="B100" t="str">
+        <f t="shared" si="6"/>
+        <v>mcuenta_debitos_automaticos_avg_3</v>
+      </c>
+      <c r="C100" t="str">
+        <f t="shared" si="6"/>
+        <v>mcuenta_debitos_automaticos_avg_6</v>
+      </c>
+      <c r="D100" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mcuenta_debitos_automaticos, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS mcuenta_debitos_automaticos_avg_3</v>
+      </c>
+      <c r="E100" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mcuenta_debitos_automaticos, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS mcuenta_debitos_automaticos_avg_6</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>20</v>
+      </c>
+      <c r="B101" t="str">
+        <f t="shared" si="6"/>
+        <v>mcuentas_saldo_avg_3</v>
+      </c>
+      <c r="C101" t="str">
+        <f t="shared" si="6"/>
+        <v>mcuentas_saldo_avg_6</v>
+      </c>
+      <c r="D101" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mcuentas_saldo, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS mcuentas_saldo_avg_3</v>
+      </c>
+      <c r="E101" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mcuentas_saldo, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS mcuentas_saldo_avg_6</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>83</v>
+      </c>
+      <c r="B102" t="str">
+        <f t="shared" si="6"/>
+        <v>mextraccion_autoservicio_avg_3</v>
+      </c>
+      <c r="C102" t="str">
+        <f t="shared" si="6"/>
+        <v>mextraccion_autoservicio_avg_6</v>
+      </c>
+      <c r="D102" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mextraccion_autoservicio, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS mextraccion_autoservicio_avg_3</v>
+      </c>
+      <c r="E102" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mextraccion_autoservicio, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS mextraccion_autoservicio_avg_6</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>75</v>
+      </c>
+      <c r="B103" t="str">
+        <f t="shared" si="6"/>
+        <v>mforex_buy_avg_3</v>
+      </c>
+      <c r="C103" t="str">
+        <f t="shared" si="6"/>
+        <v>mforex_buy_avg_6</v>
+      </c>
+      <c r="D103" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mforex_buy, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS mforex_buy_avg_3</v>
+      </c>
+      <c r="E103" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mforex_buy, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS mforex_buy_avg_6</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>77</v>
+      </c>
+      <c r="B104" t="str">
+        <f t="shared" si="6"/>
+        <v>mforex_sell_avg_3</v>
+      </c>
+      <c r="C104" t="str">
+        <f t="shared" si="6"/>
+        <v>mforex_sell_avg_6</v>
+      </c>
+      <c r="D104" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mforex_sell, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS mforex_sell_avg_3</v>
+      </c>
+      <c r="E104" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mforex_sell, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS mforex_sell_avg_6</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>41</v>
+      </c>
+      <c r="B105" t="str">
+        <f t="shared" si="6"/>
+        <v>minversion1_dolares_avg_3</v>
+      </c>
+      <c r="C105" t="str">
+        <f t="shared" si="6"/>
+        <v>minversion1_dolares_avg_6</v>
+      </c>
+      <c r="D105" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(minversion1_dolares, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS minversion1_dolares_avg_3</v>
+      </c>
+      <c r="E105" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(minversion1_dolares, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS minversion1_dolares_avg_6</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>40</v>
+      </c>
+      <c r="B106" t="str">
+        <f t="shared" si="6"/>
+        <v>minversion1_pesos_avg_3</v>
+      </c>
+      <c r="C106" t="str">
+        <f t="shared" si="6"/>
+        <v>minversion1_pesos_avg_6</v>
+      </c>
+      <c r="D106" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(minversion1_pesos, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS minversion1_pesos_avg_3</v>
+      </c>
+      <c r="E106" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(minversion1_pesos, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS minversion1_pesos_avg_6</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>43</v>
+      </c>
+      <c r="B107" t="str">
+        <f t="shared" si="6"/>
+        <v>minversion2_avg_3</v>
+      </c>
+      <c r="C107" t="str">
+        <f t="shared" si="6"/>
+        <v>minversion2_avg_6</v>
+      </c>
+      <c r="D107" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(minversion2, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS minversion2_avg_3</v>
+      </c>
+      <c r="E107" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(minversion2, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS minversion2_avg_6</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>60</v>
+      </c>
+      <c r="B108" t="str">
+        <f t="shared" si="6"/>
+        <v>mpagodeservicios_avg_3</v>
+      </c>
+      <c r="C108" t="str">
+        <f t="shared" si="6"/>
+        <v>mpagodeservicios_avg_6</v>
+      </c>
+      <c r="D108" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mpagodeservicios, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS mpagodeservicios_avg_3</v>
+      </c>
+      <c r="E108" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mpagodeservicios, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS mpagodeservicios_avg_6</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>62</v>
+      </c>
+      <c r="B109" t="str">
+        <f t="shared" si="6"/>
+        <v>mpagomiscuentas_avg_3</v>
+      </c>
+      <c r="C109" t="str">
+        <f t="shared" si="6"/>
+        <v>mpagomiscuentas_avg_6</v>
+      </c>
+      <c r="D109" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mpagomiscuentas, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS mpagomiscuentas_avg_3</v>
+      </c>
+      <c r="E109" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mpagomiscuentas, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS mpagomiscuentas_avg_6</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>9</v>
+      </c>
+      <c r="B110" t="str">
+        <f t="shared" si="6"/>
+        <v>mpasivos_margen_avg_3</v>
+      </c>
+      <c r="C110" t="str">
+        <f t="shared" si="6"/>
+        <v>mpasivos_margen_avg_6</v>
+      </c>
+      <c r="D110" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mpasivos_margen, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS mpasivos_margen_avg_3</v>
+      </c>
+      <c r="E110" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mpasivos_margen, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS mpasivos_margen_avg_6</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>50</v>
+      </c>
+      <c r="B111" t="str">
+        <f t="shared" si="6"/>
+        <v>mpayroll_avg_3</v>
+      </c>
+      <c r="C111" t="str">
+        <f t="shared" si="6"/>
+        <v>mpayroll_avg_6</v>
+      </c>
+      <c r="D111" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mpayroll, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS mpayroll_avg_3</v>
+      </c>
+      <c r="E111" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mpayroll, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS mpayroll_avg_6</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>51</v>
+      </c>
+      <c r="B112" t="str">
+        <f t="shared" si="6"/>
+        <v>mpayroll2_avg_3</v>
+      </c>
+      <c r="C112" t="str">
+        <f t="shared" si="6"/>
+        <v>mpayroll2_avg_6</v>
+      </c>
+      <c r="D112" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mpayroll2, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS mpayroll2_avg_3</v>
+      </c>
+      <c r="E112" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mpayroll2, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS mpayroll2_avg_6</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>37</v>
+      </c>
+      <c r="B113" t="str">
+        <f t="shared" si="6"/>
+        <v>mplazo_fijo_dolares_avg_3</v>
+      </c>
+      <c r="C113" t="str">
+        <f t="shared" si="6"/>
+        <v>mplazo_fijo_dolares_avg_6</v>
+      </c>
+      <c r="D113" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mplazo_fijo_dolares, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS mplazo_fijo_dolares_avg_3</v>
+      </c>
+      <c r="E113" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mplazo_fijo_dolares, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS mplazo_fijo_dolares_avg_6</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>38</v>
+      </c>
+      <c r="B114" t="str">
+        <f t="shared" si="6"/>
+        <v>mplazo_fijo_pesos_avg_3</v>
+      </c>
+      <c r="C114" t="str">
+        <f t="shared" si="6"/>
+        <v>mplazo_fijo_pesos_avg_6</v>
+      </c>
+      <c r="D114" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mplazo_fijo_pesos, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS mplazo_fijo_pesos_avg_3</v>
+      </c>
+      <c r="E114" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mplazo_fijo_pesos, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS mplazo_fijo_pesos_avg_6</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>35</v>
+      </c>
+      <c r="B115" t="str">
+        <f t="shared" si="6"/>
+        <v>mprestamos_hipotecarios_avg_3</v>
+      </c>
+      <c r="C115" t="str">
+        <f t="shared" si="6"/>
+        <v>mprestamos_hipotecarios_avg_6</v>
+      </c>
+      <c r="D115" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mprestamos_hipotecarios, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS mprestamos_hipotecarios_avg_3</v>
+      </c>
+      <c r="E115" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mprestamos_hipotecarios, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS mprestamos_hipotecarios_avg_6</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>31</v>
+      </c>
+      <c r="B116" t="str">
+        <f t="shared" si="6"/>
+        <v>mprestamos_personales_avg_3</v>
+      </c>
+      <c r="C116" t="str">
+        <f t="shared" si="6"/>
+        <v>mprestamos_personales_avg_6</v>
+      </c>
+      <c r="D116" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mprestamos_personales, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS mprestamos_personales_avg_3</v>
+      </c>
+      <c r="E116" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mprestamos_personales, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS mprestamos_personales_avg_6</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>33</v>
+      </c>
+      <c r="B117" t="str">
+        <f t="shared" si="6"/>
+        <v>mprestamos_prendarios_avg_3</v>
+      </c>
+      <c r="C117" t="str">
+        <f t="shared" si="6"/>
+        <v>mprestamos_prendarios_avg_6</v>
+      </c>
+      <c r="D117" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mprestamos_prendarios, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS mprestamos_prendarios_avg_3</v>
+      </c>
+      <c r="E117" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mprestamos_prendarios, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS mprestamos_prendarios_avg_6</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>5</v>
+      </c>
+      <c r="B118" t="str">
+        <f t="shared" si="6"/>
+        <v>mrentabilidad_avg_3</v>
+      </c>
+      <c r="C118" t="str">
+        <f t="shared" si="6"/>
+        <v>mrentabilidad_avg_6</v>
+      </c>
+      <c r="D118" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mrentabilidad, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS mrentabilidad_avg_3</v>
+      </c>
+      <c r="E118" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mrentabilidad, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS mrentabilidad_avg_6</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>6</v>
+      </c>
+      <c r="B119" t="str">
+        <f t="shared" si="6"/>
+        <v>mrentabilidad_annual_avg_3</v>
+      </c>
+      <c r="C119" t="str">
+        <f t="shared" si="6"/>
+        <v>mrentabilidad_annual_avg_6</v>
+      </c>
+      <c r="D119" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mrentabilidad_annual, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS mrentabilidad_annual_avg_3</v>
+      </c>
+      <c r="E119" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mrentabilidad_annual, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS mrentabilidad_annual_avg_6</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>29</v>
+      </c>
+      <c r="B120" t="str">
+        <f t="shared" si="6"/>
+        <v>mtarjeta_master_consumo_avg_3</v>
+      </c>
+      <c r="C120" t="str">
+        <f t="shared" si="6"/>
+        <v>mtarjeta_master_consumo_avg_6</v>
+      </c>
+      <c r="D120" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mtarjeta_master_consumo, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS mtarjeta_master_consumo_avg_3</v>
+      </c>
+      <c r="E120" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mtarjeta_master_consumo, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS mtarjeta_master_consumo_avg_6</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>68</v>
+      </c>
+      <c r="B121" t="str">
+        <f t="shared" si="6"/>
+        <v>mtarjeta_master_descuentos_avg_3</v>
+      </c>
+      <c r="C121" t="str">
+        <f t="shared" si="6"/>
+        <v>mtarjeta_master_descuentos_avg_6</v>
+      </c>
+      <c r="D121" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mtarjeta_master_descuentos, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS mtarjeta_master_descuentos_avg_3</v>
+      </c>
+      <c r="E121" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mtarjeta_master_descuentos, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS mtarjeta_master_descuentos_avg_6</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>26</v>
+      </c>
+      <c r="B122" t="str">
+        <f t="shared" si="6"/>
+        <v>mtarjeta_visa_consumo_avg_3</v>
+      </c>
+      <c r="C122" t="str">
+        <f t="shared" si="6"/>
+        <v>mtarjeta_visa_consumo_avg_6</v>
+      </c>
+      <c r="D122" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mtarjeta_visa_consumo, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS mtarjeta_visa_consumo_avg_3</v>
+      </c>
+      <c r="E122" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mtarjeta_visa_consumo, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS mtarjeta_visa_consumo_avg_6</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>66</v>
+      </c>
+      <c r="B123" t="str">
+        <f t="shared" si="6"/>
+        <v>mtarjeta_visa_descuentos_avg_3</v>
+      </c>
+      <c r="C123" t="str">
+        <f t="shared" si="6"/>
+        <v>mtarjeta_visa_descuentos_avg_6</v>
+      </c>
+      <c r="D123" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mtarjeta_visa_descuentos, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS mtarjeta_visa_descuentos_avg_3</v>
+      </c>
+      <c r="E123" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mtarjeta_visa_descuentos, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS mtarjeta_visa_descuentos_avg_6</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>81</v>
+      </c>
+      <c r="B124" t="str">
+        <f t="shared" si="6"/>
+        <v>mtransferencias_emitidas_avg_3</v>
+      </c>
+      <c r="C124" t="str">
+        <f t="shared" si="6"/>
+        <v>mtransferencias_emitidas_avg_6</v>
+      </c>
+      <c r="D124" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mtransferencias_emitidas, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS mtransferencias_emitidas_avg_3</v>
+      </c>
+      <c r="E124" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mtransferencias_emitidas, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS mtransferencias_emitidas_avg_6</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>79</v>
+      </c>
+      <c r="B125" t="str">
+        <f t="shared" si="6"/>
+        <v>mtransferencias_recibidas_avg_3</v>
+      </c>
+      <c r="C125" t="str">
+        <f t="shared" si="6"/>
+        <v>mtransferencias_recibidas_avg_6</v>
+      </c>
+      <c r="D125" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mtransferencias_recibidas, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS mtransferencias_recibidas_avg_3</v>
+      </c>
+      <c r="E125" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mtransferencias_recibidas, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS mtransferencias_recibidas_avg_6</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>58</v>
+      </c>
+      <c r="B126" t="str">
+        <f t="shared" si="6"/>
+        <v>mttarjeta_master_debitos_automaticos_avg_3</v>
+      </c>
+      <c r="C126" t="str">
+        <f t="shared" si="6"/>
+        <v>mttarjeta_master_debitos_automaticos_avg_6</v>
+      </c>
+      <c r="D126" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mttarjeta_master_debitos_automaticos, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS mttarjeta_master_debitos_automaticos_avg_3</v>
+      </c>
+      <c r="E126" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mttarjeta_master_debitos_automaticos, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS mttarjeta_master_debitos_automaticos_avg_6</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>56</v>
+      </c>
+      <c r="B127" t="str">
+        <f t="shared" si="6"/>
+        <v>mttarjeta_visa_debitos_automaticos_avg_3</v>
+      </c>
+      <c r="C127" t="str">
+        <f t="shared" si="6"/>
+        <v>mttarjeta_visa_debitos_automaticos_avg_6</v>
+      </c>
+      <c r="D127" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mttarjeta_visa_debitos_automaticos, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS mttarjeta_visa_debitos_automaticos_avg_3</v>
+      </c>
+      <c r="E127" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(mttarjeta_visa_debitos_automaticos, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS mttarjeta_visa_debitos_automaticos_avg_6</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>92</v>
+      </c>
+      <c r="B128" t="str">
+        <f t="shared" si="6"/>
+        <v>tcallcenter_avg_3</v>
+      </c>
+      <c r="C128" t="str">
+        <f t="shared" si="6"/>
+        <v>tcallcenter_avg_6</v>
+      </c>
+      <c r="D128" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(tcallcenter, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS tcallcenter_avg_3</v>
+      </c>
+      <c r="E128" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(tcallcenter, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS tcallcenter_avg_6</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>11</v>
+      </c>
+      <c r="B129" t="str">
+        <f t="shared" si="6"/>
+        <v>tcuentas_avg_3</v>
+      </c>
+      <c r="C129" t="str">
+        <f t="shared" si="6"/>
+        <v>tcuentas_avg_6</v>
+      </c>
+      <c r="D129" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(tcuentas, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS tcuentas_avg_3</v>
+      </c>
+      <c r="E129" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(tcuentas, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS tcuentas_avg_6</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>94</v>
+      </c>
+      <c r="B130" t="str">
+        <f t="shared" si="6"/>
+        <v>thomebanking_avg_3</v>
+      </c>
+      <c r="C130" t="str">
+        <f t="shared" si="6"/>
+        <v>thomebanking_avg_6</v>
+      </c>
+      <c r="D130" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(thomebanking, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS thomebanking_avg_3</v>
+      </c>
+      <c r="E130" t="str">
+        <f t="shared" si="5"/>
+        <v>,AVG(thomebanking, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS thomebanking_avg_6</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>106</v>
+      </c>
+      <c r="B131" t="str">
+        <f t="shared" ref="B131:C153" si="7">_xlfn.CONCAT($A131,"_avg_",B$1)</f>
+        <v>tmobile_app_avg_3</v>
+      </c>
+      <c r="C131" t="str">
+        <f t="shared" si="7"/>
+        <v>tmobile_app_avg_6</v>
+      </c>
+      <c r="D131" t="str">
+        <f t="shared" ref="D131:E153" si="8">",AVG(" &amp;$A131 &amp;", " &amp;B$1 &amp;") OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN " &amp;B$1 &amp; " PRECEDING AND CURRENT ROW) AS " &amp;B131</f>
+        <v>,AVG(tmobile_app, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS tmobile_app_avg_3</v>
+      </c>
+      <c r="E131" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(tmobile_app, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS tmobile_app_avg_6</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>150</v>
+      </c>
+      <c r="B132" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_cadelantosefectivo_avg_3</v>
+      </c>
+      <c r="C132" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_cadelantosefectivo_avg_6</v>
+      </c>
+      <c r="D132" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_cadelantosefectivo, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Visa_cadelantosefectivo_avg_3</v>
+      </c>
+      <c r="E132" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_cadelantosefectivo, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Visa_cadelantosefectivo_avg_6</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>149</v>
+      </c>
+      <c r="B133" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_cconsumos_avg_3</v>
+      </c>
+      <c r="C133" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_cconsumos_avg_6</v>
+      </c>
+      <c r="D133" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_cconsumos, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Visa_cconsumos_avg_3</v>
+      </c>
+      <c r="E133" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_cconsumos, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Visa_cconsumos_avg_6</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>130</v>
+      </c>
+      <c r="B134" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_delinquency_avg_3</v>
+      </c>
+      <c r="C134" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_delinquency_avg_6</v>
+      </c>
+      <c r="D134" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_delinquency, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Visa_delinquency_avg_3</v>
+      </c>
+      <c r="E134" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_delinquency, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Visa_delinquency_avg_6</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>147</v>
+      </c>
+      <c r="B135" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_fechaalta_avg_3</v>
+      </c>
+      <c r="C135" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_fechaalta_avg_6</v>
+      </c>
+      <c r="D135" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_fechaalta, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Visa_fechaalta_avg_3</v>
+      </c>
+      <c r="E135" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_fechaalta, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Visa_fechaalta_avg_6</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>134</v>
+      </c>
+      <c r="B136" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_Finiciomora_avg_3</v>
+      </c>
+      <c r="C136" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_Finiciomora_avg_6</v>
+      </c>
+      <c r="D136" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_Finiciomora, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Visa_Finiciomora_avg_3</v>
+      </c>
+      <c r="E136" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_Finiciomora, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Visa_Finiciomora_avg_6</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>143</v>
+      </c>
+      <c r="B137" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_fultimo_cierre_avg_3</v>
+      </c>
+      <c r="C137" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_fultimo_cierre_avg_6</v>
+      </c>
+      <c r="D137" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_fultimo_cierre, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Visa_fultimo_cierre_avg_3</v>
+      </c>
+      <c r="E137" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_fultimo_cierre, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Visa_fultimo_cierre_avg_6</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>133</v>
+      </c>
+      <c r="B138" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_Fvencimiento_avg_3</v>
+      </c>
+      <c r="C138" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_Fvencimiento_avg_6</v>
+      </c>
+      <c r="D138" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_Fvencimiento, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Visa_Fvencimiento_avg_3</v>
+      </c>
+      <c r="E138" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_Fvencimiento, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Visa_Fvencimiento_avg_6</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>142</v>
+      </c>
+      <c r="B139" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_madelantodolares_avg_3</v>
+      </c>
+      <c r="C139" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_madelantodolares_avg_6</v>
+      </c>
+      <c r="D139" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_madelantodolares, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Visa_madelantodolares_avg_3</v>
+      </c>
+      <c r="E139" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_madelantodolares, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Visa_madelantodolares_avg_6</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>141</v>
+      </c>
+      <c r="B140" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_madelantopesos_avg_3</v>
+      </c>
+      <c r="C140" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_madelantopesos_avg_6</v>
+      </c>
+      <c r="D140" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_madelantopesos, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Visa_madelantopesos_avg_3</v>
+      </c>
+      <c r="E140" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_madelantopesos, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Visa_madelantopesos_avg_6</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>139</v>
+      </c>
+      <c r="B141" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_mconsumosdolares_avg_3</v>
+      </c>
+      <c r="C141" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_mconsumosdolares_avg_6</v>
+      </c>
+      <c r="D141" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_mconsumosdolares, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Visa_mconsumosdolares_avg_3</v>
+      </c>
+      <c r="E141" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_mconsumosdolares, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Visa_mconsumosdolares_avg_6</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>138</v>
+      </c>
+      <c r="B142" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_mconsumospesos_avg_3</v>
+      </c>
+      <c r="C142" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_mconsumospesos_avg_6</v>
+      </c>
+      <c r="D142" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_mconsumospesos, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Visa_mconsumospesos_avg_3</v>
+      </c>
+      <c r="E142" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_mconsumospesos, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Visa_mconsumospesos_avg_6</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>148</v>
+      </c>
+      <c r="B143" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_mconsumototal_avg_3</v>
+      </c>
+      <c r="C143" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_mconsumototal_avg_6</v>
+      </c>
+      <c r="D143" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_mconsumototal, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Visa_mconsumototal_avg_3</v>
+      </c>
+      <c r="E143" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_mconsumototal, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Visa_mconsumototal_avg_6</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>132</v>
+      </c>
+      <c r="B144" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_mfinanciacion_limite_avg_3</v>
+      </c>
+      <c r="C144" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_mfinanciacion_limite_avg_6</v>
+      </c>
+      <c r="D144" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_mfinanciacion_limite, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Visa_mfinanciacion_limite_avg_3</v>
+      </c>
+      <c r="E144" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_mfinanciacion_limite, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Visa_mfinanciacion_limite_avg_6</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>140</v>
+      </c>
+      <c r="B145" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_mlimitecompra_avg_3</v>
+      </c>
+      <c r="C145" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_mlimitecompra_avg_6</v>
+      </c>
+      <c r="D145" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_mlimitecompra, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Visa_mlimitecompra_avg_3</v>
+      </c>
+      <c r="E145" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_mlimitecompra, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Visa_mlimitecompra_avg_6</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>144</v>
+      </c>
+      <c r="B146" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_mpagado_avg_3</v>
+      </c>
+      <c r="C146" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_mpagado_avg_6</v>
+      </c>
+      <c r="D146" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_mpagado, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Visa_mpagado_avg_3</v>
+      </c>
+      <c r="E146" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_mpagado, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Visa_mpagado_avg_6</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>151</v>
+      </c>
+      <c r="B147" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_mpagominimo_avg_3</v>
+      </c>
+      <c r="C147" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_mpagominimo_avg_6</v>
+      </c>
+      <c r="D147" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_mpagominimo, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Visa_mpagominimo_avg_3</v>
+      </c>
+      <c r="E147" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_mpagominimo, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Visa_mpagominimo_avg_6</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>146</v>
+      </c>
+      <c r="B148" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_mpagosdolares_avg_3</v>
+      </c>
+      <c r="C148" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_mpagosdolares_avg_6</v>
+      </c>
+      <c r="D148" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_mpagosdolares, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Visa_mpagosdolares_avg_3</v>
+      </c>
+      <c r="E148" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_mpagosdolares, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Visa_mpagosdolares_avg_6</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>145</v>
+      </c>
+      <c r="B149" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_mpagospesos_avg_3</v>
+      </c>
+      <c r="C149" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_mpagospesos_avg_6</v>
+      </c>
+      <c r="D149" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_mpagospesos, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Visa_mpagospesos_avg_3</v>
+      </c>
+      <c r="E149" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_mpagospesos, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Visa_mpagospesos_avg_6</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>137</v>
+      </c>
+      <c r="B150" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_msaldodolares_avg_3</v>
+      </c>
+      <c r="C150" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_msaldodolares_avg_6</v>
+      </c>
+      <c r="D150" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_msaldodolares, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Visa_msaldodolares_avg_3</v>
+      </c>
+      <c r="E150" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_msaldodolares, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Visa_msaldodolares_avg_6</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>136</v>
+      </c>
+      <c r="B151" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_msaldopesos_avg_3</v>
+      </c>
+      <c r="C151" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_msaldopesos_avg_6</v>
+      </c>
+      <c r="D151" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_msaldopesos, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Visa_msaldopesos_avg_3</v>
+      </c>
+      <c r="E151" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_msaldopesos, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Visa_msaldopesos_avg_6</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>135</v>
+      </c>
+      <c r="B152" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_msaldototal_avg_3</v>
+      </c>
+      <c r="C152" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_msaldototal_avg_6</v>
+      </c>
+      <c r="D152" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_msaldototal, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Visa_msaldototal_avg_3</v>
+      </c>
+      <c r="E152" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_msaldototal, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Visa_msaldototal_avg_6</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>131</v>
+      </c>
+      <c r="B153" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_status_avg_3</v>
+      </c>
+      <c r="C153" t="str">
+        <f t="shared" si="7"/>
+        <v>Visa_status_avg_6</v>
+      </c>
+      <c r="D153" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_status, 3) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 3 PRECEDING AND CURRENT ROW) AS Visa_status_avg_3</v>
+      </c>
+      <c r="E153" t="str">
+        <f t="shared" si="8"/>
+        <v>,AVG(Visa_status, 6) OVER (PARTITION BY numero_de_cliente ORDER BY foto_mes ASC ROWS BETWEEN 6 PRECEDING AND CURRENT ROW) AS Visa_status_avg_6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>